<commit_message>
Finshing the table view
</commit_message>
<xml_diff>
--- a/Excel/Data_Excel.xlsx
+++ b/Excel/Data_Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Swimmer_ID"/>
@@ -109,7 +109,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +122,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -158,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -172,6 +178,36 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
@@ -181,34 +217,7 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -219,6 +228,9 @@
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -529,9 +541,9 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="12" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="22" width="19.290714285714284" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="12" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="22" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -667,7 +679,7 @@
   </sheetPr>
   <dimension ref="A1:N226"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -680,15 +692,15 @@
     <col min="7" max="7" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="12" width="14.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="12" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="20" width="18.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="12" width="21.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="12" width="22.005" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="21" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="12" width="19.005" customWidth="1" bestFit="1"/>
     <col min="14" max="14" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -697,16 +709,16 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="18" t="s">
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -721,13 +733,13 @@
       <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="20" t="s">
         <v>15</v>
       </c>
     </row>
@@ -10643,7 +10655,7 @@
   </sheetPr>
   <dimension ref="A1:FN226"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10679,7 +10691,7 @@
     <col min="30" max="30" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="31" max="31" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="32" max="32" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="16" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="34" max="34" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="35" max="35" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="36" max="36" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
@@ -10816,7 +10828,7 @@
     <col min="167" max="167" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="168" max="168" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="169" max="169" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="170" max="170" style="16" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="170" max="170" style="17" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">

</xml_diff>